<commit_message>
filling in the report
</commit_message>
<xml_diff>
--- a/LTSpice/final_project_pss.xlsx
+++ b/LTSpice/final_project_pss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imecinternational-my.sharepoint.com/personal/mouras54_imec_be/Documents/VUB cursus analoge elektronica/AEC_2020_21_STUDENTS/LTSpice/final project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUB\MA1\Analog Electronics\Analog_electronics_project\LTSpice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="11_F25DC773A252ABDACC1048D9395C6A0A5ADE58F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D51D54B5-62CA-4EB5-8C0E-79943E1CF914}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928AFEC9-0F10-41F0-9B44-2F435988F9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Vin (V)</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Gain (dB)</t>
+  </si>
+  <si>
+    <t>Vout(V)</t>
+  </si>
+  <si>
+    <t>vout*vin</t>
+  </si>
+  <si>
+    <t>DB</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -217,7 +226,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -226,7 +234,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -244,7 +252,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -306,7 +314,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -382,7 +390,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-BE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -451,52 +459,52 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>123.01029995663981</c:v>
+                  <c:v>-5.0397000433601988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116.34377314857073</c:v>
+                  <c:v>4.5307731485707308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109.67713286085319</c:v>
+                  <c:v>53.07713286085319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>103.01029995663981</c:v>
+                  <c:v>54.010299956639813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.343773148570733</c:v>
+                  <c:v>54.843773148570733</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.677132860853192</c:v>
+                  <c:v>55.177132860853192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>83.010299956639813</c:v>
+                  <c:v>55.31029995663981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76.343773148570733</c:v>
+                  <c:v>55.243773148570732</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69.677132860853177</c:v>
+                  <c:v>54.87713286085318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63.010299956639813</c:v>
+                  <c:v>53.31029995663981</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>56.343773148570733</c:v>
+                  <c:v>48.943773148570735</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49.677132860853177</c:v>
+                  <c:v>43.177132860853177</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43.010299956639813</c:v>
+                  <c:v>36.710299956639815</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.343773148570733</c:v>
+                  <c:v>30.043773148570732</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.677132860853185</c:v>
+                  <c:v>23.477132860853185</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.010299956639813</c:v>
+                  <c:v>16.810299956639813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -591,7 +599,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-BE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -629,7 +637,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="824678456"/>
@@ -709,7 +717,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-BE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -747,7 +755,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="824679440"/>
@@ -795,7 +803,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -809,7 +817,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -871,13 +879,23 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1210550506447336"/>
+          <c:y val="6.464487130257543E-2"/>
+          <c:w val="0.85200173679556856"/>
+          <c:h val="0.88968186373226787"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -947,7 +965,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-BE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1016,52 +1034,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-128.05000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-111.813</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-56.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-41.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-34.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-27.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-21.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-14.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-9.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-7.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-6.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>-6.3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-6.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-6.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>-6.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,7 +1174,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-BE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1194,7 +1212,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="824678456"/>
@@ -1274,7 +1292,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-BE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1312,12 +1330,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="824679440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1360,7 +1379,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2529,10 +2548,10 @@
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2823,10 +2842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:F18"/>
+  <dimension ref="C1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,280 +2868,515 @@
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <f>0.000001</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <f>20*LOG10(C3/SQRT(2))</f>
         <v>-123.01029995663981</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>-128.05000000000001</v>
       </c>
       <c r="F3" s="1">
         <f>E3-D3</f>
-        <v>123.01029995663981</v>
+        <v>-5.0397000433601988</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f>0.0000021544</f>
         <v>2.1544000000000001E-6</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <f t="shared" ref="D4:D18" si="0">20*LOG10(C4/SQRT(2))</f>
         <v>-116.34377314857073</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>-111.813</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F18" si="1">E4-D4</f>
-        <v>116.34377314857073</v>
+        <v>4.5307731485707308</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <f>0.0000046415</f>
         <v>4.6415000000000004E-6</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>-109.67713286085319</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>-56.6</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>109.67713286085319</v>
+        <v>53.07713286085319</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f>10*C3</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>-103.01029995663981</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
+        <v>-49</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>103.01029995663981</v>
+        <v>54.010299956639813</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <f t="shared" ref="C7:C18" si="2">10*C4</f>
         <v>2.1544000000000002E-5</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>-96.343773148570733</v>
       </c>
       <c r="E7" s="5">
-        <v>0</v>
+        <v>-41.5</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>96.343773148570733</v>
+        <v>54.843773148570733</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <f t="shared" si="2"/>
         <v>4.6415000000000002E-5</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>-89.677132860853192</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>-34.5</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>89.677132860853192</v>
+        <v>55.177132860853192</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <f t="shared" si="2"/>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>-83.010299956639813</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>-27.7</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>83.010299956639813</v>
+        <v>55.31029995663981</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f t="shared" si="2"/>
         <v>2.1544000000000001E-4</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>-76.343773148570733</v>
       </c>
       <c r="E10" s="5">
-        <v>0</v>
+        <v>-21.1</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>76.343773148570733</v>
+        <v>55.243773148570732</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <f t="shared" si="2"/>
         <v>4.6415000000000003E-4</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>-69.677132860853177</v>
       </c>
       <c r="E11" s="5">
-        <v>0</v>
+        <v>-14.8</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>69.677132860853177</v>
+        <v>54.87713286085318</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>-63.010299956639813</v>
       </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>63.010299956639813</v>
+        <v>53.31029995663981</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <f t="shared" si="2"/>
         <v>2.1543999999999999E-3</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>-56.343773148570733</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
+        <v>-7.4</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>56.343773148570733</v>
+        <v>48.943773148570735</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <f t="shared" si="2"/>
         <v>4.6415000000000007E-3</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>-49.677132860853177</v>
       </c>
       <c r="E14" s="5">
-        <v>0</v>
+        <v>-6.5</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="1"/>
-        <v>49.677132860853177</v>
+        <v>43.177132860853177</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>-43.010299956639813</v>
       </c>
       <c r="E15" s="5">
-        <v>0</v>
+        <v>-6.3</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>43.010299956639813</v>
+        <v>36.710299956639815</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <f t="shared" si="2"/>
         <v>2.1544000000000001E-2</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <f t="shared" si="0"/>
         <v>-36.343773148570733</v>
       </c>
       <c r="E16" s="5">
-        <v>0</v>
+        <v>-6.3</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>36.343773148570733</v>
+        <v>30.043773148570732</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <f t="shared" si="2"/>
         <v>4.6415000000000005E-2</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>-29.677132860853185</v>
       </c>
       <c r="E17" s="5">
-        <v>0</v>
+        <v>-6.2</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
-        <v>29.677132860853185</v>
+        <v>23.477132860853185</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <f t="shared" si="0"/>
         <v>-23.010299956639813</v>
       </c>
       <c r="E18" s="6">
-        <v>0</v>
+        <v>-6.2</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>23.010299956639813</v>
+        <v>16.810299956639813</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>10^(E3/20)</f>
+        <v>3.9582206483572143E-7</v>
+      </c>
+      <c r="E24">
+        <f>D24*C4</f>
+        <v>8.5275905648207824E-13</v>
+      </c>
+      <c r="F24">
+        <f xml:space="preserve"> 20*LOG10(E24)</f>
+        <v>-241.38347319193093</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" ref="D25:D40" si="3">10^(E4/20)</f>
+        <v>2.5665515994850496E-6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:E39" si="4">D25*C5</f>
+        <v>1.1912649249009858E-11</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F39" si="5" xml:space="preserve"> 20*LOG10(E25)</f>
+        <v>-218.4798329042134</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>1.4791083881682066E-3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>1.4791083881682064E-8</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>-156.6</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>3.5481338923357528E-3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>7.6440996576481467E-8</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>-142.33347319193092</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>8.4139514164519452E-3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>3.9053355499461707E-7</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>-128.16683290421338</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>1.8836490894897997E-2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>1.8836490894897995E-6</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>-114.50000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>4.1209751909733E-2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>8.8782289514328775E-6</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>-101.03347319193092</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>8.8104887300801349E-2</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>4.0893883440666951E-5</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="5"/>
+        <v>-87.766832904213373</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>0.18197008586099833</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>1.8197008586099835E-4</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="5"/>
+        <v>-74.800000000000011</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>0.32734069487883821</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>7.0522279304696906E-4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="5"/>
+        <v>-63.033473191930923</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>0.42657951880159267</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>1.9799688365175925E-3</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="5"/>
+        <v>-54.066832904213371</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>0.47315125896148047</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>4.7315125896148051E-3</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="5"/>
+        <v>-46.5</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>0.48417236758409932</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>1.0431009487231836E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="5"/>
+        <v>-39.633473191930918</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>0.48417236758409932</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="4"/>
+        <v>2.2472860441415971E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="5"/>
+        <v>-32.966832904213369</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>0.48977881936844614</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="4"/>
+        <v>4.8977881936844617E-2</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="5"/>
+        <v>-26.200000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>0.48977881936844614</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>